<commit_message>
Version with good round values
</commit_message>
<xml_diff>
--- a/settings/prices.xlsx
+++ b/settings/prices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtr42\cropio\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C6D71E-50E5-455A-B64D-06085990DA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E573A1EE-06FB-410C-9997-09EF084DA038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,6 +160,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -192,7 +195,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -476,7 +479,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D42" sqref="D39:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>